<commit_message>
added pin headers to bom
</commit_message>
<xml_diff>
--- a/Full BOM - DigiKey.xlsx
+++ b/Full BOM - DigiKey.xlsx
@@ -328,7 +328,7 @@
         </is>
       </c>
       <c t="n" r="K2">
-        <v>307436</v>
+        <v>307398</v>
       </c>
       <c t="inlineStr" r="L2">
         <is>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c t="n" r="K5">
-        <v>258650</v>
+        <v>279650</v>
       </c>
       <c t="inlineStr" r="L5">
         <is>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c t="n" r="K8">
-        <v>98345</v>
+        <v>98305</v>
       </c>
       <c t="inlineStr" r="L8">
         <is>
@@ -1964,7 +1964,7 @@
         </is>
       </c>
       <c t="n" r="K23">
-        <v>1804532</v>
+        <v>1804032</v>
       </c>
       <c t="inlineStr" r="L23">
         <is>
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c t="n" r="K25">
-        <v>210163</v>
+        <v>209885</v>
       </c>
       <c t="inlineStr" r="L25">
         <is>
@@ -2611,6 +2611,240 @@
         </is>
       </c>
       <c t="inlineStr" r="P31">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c t="inlineStr" r="A32">
+        <is>
+          <t>SSW-104-01-G-D</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B32">
+        <is>
+          <t>Samtec Inc.</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C32">
+        <is>
+          <t>SAM1208-04-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D32">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="E32">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="F32">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G32">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H32">
+        <v>1</v>
+      </c>
+      <c t="inlineStr" r="I32">
+        <is>
+          <t>1,16000</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J32">
+        <is>
+          <t>1,16 €</t>
+        </is>
+      </c>
+      <c t="n" r="K32">
+        <v>2898</v>
+      </c>
+      <c t="inlineStr" r="L32">
+        <is>
+          <t>2 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M32">
+        <is>
+          <t>CONN RCPT 8POS 0.1 GOLD PCB</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N32">
+        <is>
+          <t>ROHS3 Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O32">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P32">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c t="inlineStr" r="A33">
+        <is>
+          <t>TSW-104-17-G-D</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B33">
+        <is>
+          <t>Samtec Inc.</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C33">
+        <is>
+          <t>SAM1060-04-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D33">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="E33">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="F33">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G33">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H33">
+        <v>1</v>
+      </c>
+      <c t="inlineStr" r="I33">
+        <is>
+          <t>0,90000</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J33">
+        <is>
+          <t>0,90 €</t>
+        </is>
+      </c>
+      <c t="n" r="K33">
+        <v>414</v>
+      </c>
+      <c t="inlineStr" r="L33">
+        <is>
+          <t>2 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M33">
+        <is>
+          <t>CONN HEADER VERT 8POS 2.54MM</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N33">
+        <is>
+          <t>ROHS3 Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O33">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P33">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c t="inlineStr" r="A34">
+        <is>
+          <t>PH1-10-UA</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B34">
+        <is>
+          <t>Adam Tech</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C34">
+        <is>
+          <t>2057-PH1-10-UA-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D34">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="E34">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c t="inlineStr" r="F34">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G34">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H34">
+        <v>1</v>
+      </c>
+      <c t="inlineStr" r="I34">
+        <is>
+          <t>0,16000</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J34">
+        <is>
+          <t>0,16 €</t>
+        </is>
+      </c>
+      <c t="n" r="K34">
+        <v>3470</v>
+      </c>
+      <c t="inlineStr" r="L34">
+        <is>
+          <t>9 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M34">
+        <is>
+          <t>CONN HEADER VERT 10POS 2.54MM</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N34">
+        <is>
+          <t>ROHS3 Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O34">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P34">
         <is>
           <t>REACH Unaffected</t>
         </is>

</xml_diff>